<commit_message>
Modifications to scripts of processing RMS attributes
1. Update scripts of processing RMS attributes. The scripts prefix “p”
stands for phase. See the auxiliary document for details.
2. Update the scripts of aggregating counterfactual simulations.
</commit_message>
<xml_diff>
--- a/SAS/Retail_attributes_RMS/retail_attributes_rms_log.xlsx
+++ b/SAS/Retail_attributes_RMS/retail_attributes_rms_log.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="0" windowWidth="31880" windowHeight="19100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
   <si>
     <t>department_code</t>
   </si>
@@ -388,13 +388,16 @@
   </si>
   <si>
     <t>n_upc</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -418,6 +421,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -436,7 +452,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -466,12 +482,113 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="129">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -486,6 +603,56 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -500,6 +667,56 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -831,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -891,6 +1108,12 @@
       <c r="F2" s="1">
         <v>42341</v>
       </c>
+      <c r="G2" s="1">
+        <v>42373</v>
+      </c>
+      <c r="H2" s="1">
+        <v>42378</v>
+      </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
@@ -911,6 +1134,12 @@
       <c r="F3" s="1">
         <v>42341</v>
       </c>
+      <c r="G3" s="1">
+        <v>42373</v>
+      </c>
+      <c r="H3" s="1">
+        <v>42378</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
@@ -931,6 +1160,12 @@
       <c r="F4" s="1">
         <v>42341</v>
       </c>
+      <c r="G4" s="1">
+        <v>42373</v>
+      </c>
+      <c r="H4" s="1">
+        <v>42378</v>
+      </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
@@ -951,6 +1186,12 @@
       <c r="F5" s="1">
         <v>42341</v>
       </c>
+      <c r="G5" s="1">
+        <v>42373</v>
+      </c>
+      <c r="H5" s="1">
+        <v>42378</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
@@ -971,6 +1212,12 @@
       <c r="F6" s="1">
         <v>42341</v>
       </c>
+      <c r="G6" s="1">
+        <v>42373</v>
+      </c>
+      <c r="H6" s="1">
+        <v>42378</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
@@ -991,6 +1238,12 @@
       <c r="F7" s="1">
         <v>42341</v>
       </c>
+      <c r="G7" s="1">
+        <v>42373</v>
+      </c>
+      <c r="H7" s="1">
+        <v>42378</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
@@ -1011,6 +1264,12 @@
       <c r="F8" s="1">
         <v>42341</v>
       </c>
+      <c r="G8" s="1">
+        <v>42373</v>
+      </c>
+      <c r="H8" s="1">
+        <v>42378</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9">
@@ -1031,6 +1290,12 @@
       <c r="F9" s="1">
         <v>42341</v>
       </c>
+      <c r="G9" s="1">
+        <v>42373</v>
+      </c>
+      <c r="H9" s="1">
+        <v>42378</v>
+      </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10">
@@ -1051,6 +1316,12 @@
       <c r="F10" s="1">
         <v>42342</v>
       </c>
+      <c r="G10" s="1">
+        <v>42373</v>
+      </c>
+      <c r="H10" s="1">
+        <v>42378</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11">
@@ -1071,6 +1342,12 @@
       <c r="F11" s="1">
         <v>42342</v>
       </c>
+      <c r="G11" s="1">
+        <v>42373</v>
+      </c>
+      <c r="H11" s="1">
+        <v>42378</v>
+      </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12">
@@ -1091,6 +1368,12 @@
       <c r="F12" s="1">
         <v>42342</v>
       </c>
+      <c r="G12" s="1">
+        <v>42374</v>
+      </c>
+      <c r="H12" s="1">
+        <v>42379</v>
+      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13">
@@ -1111,6 +1394,12 @@
       <c r="F13" s="1">
         <v>42344</v>
       </c>
+      <c r="G13" s="1">
+        <v>42374</v>
+      </c>
+      <c r="H13" s="1">
+        <v>42379</v>
+      </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14">
@@ -1131,6 +1420,12 @@
       <c r="F14" s="1">
         <v>42344</v>
       </c>
+      <c r="G14" s="1">
+        <v>42374</v>
+      </c>
+      <c r="H14" s="1">
+        <v>42379</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15">
@@ -1151,6 +1446,12 @@
       <c r="F15" s="1">
         <v>42344</v>
       </c>
+      <c r="G15" s="1">
+        <v>42374</v>
+      </c>
+      <c r="H15" s="1">
+        <v>42379</v>
+      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16">
@@ -1171,8 +1472,14 @@
       <c r="F16" s="1">
         <v>42344</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="1">
+        <v>42374</v>
+      </c>
+      <c r="H16" s="1">
+        <v>42379</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>0</v>
       </c>
@@ -1191,8 +1498,14 @@
       <c r="F17" s="1">
         <v>42344</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" s="1">
+        <v>42374</v>
+      </c>
+      <c r="H17" s="1">
+        <v>42379</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1211,8 +1524,14 @@
       <c r="F18" s="1">
         <v>42345</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="1">
+        <v>42374</v>
+      </c>
+      <c r="H18" s="1">
+        <v>42379</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>0</v>
       </c>
@@ -1231,8 +1550,14 @@
       <c r="F19" s="1">
         <v>42345</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" s="1">
+        <v>42374</v>
+      </c>
+      <c r="H19" s="1">
+        <v>42379</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1248,8 +1573,14 @@
       <c r="E20">
         <v>4873</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="F20" s="1">
+        <v>42345</v>
+      </c>
+      <c r="G20" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1265,8 +1596,14 @@
       <c r="E21">
         <v>116332</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="F21" s="1">
+        <v>42345</v>
+      </c>
+      <c r="G21" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1282,8 +1619,14 @@
       <c r="E22">
         <v>11240</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="F22" s="1">
+        <v>42345</v>
+      </c>
+      <c r="G22" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1299,8 +1642,14 @@
       <c r="E23">
         <v>6481</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="F23" s="1">
+        <v>42345</v>
+      </c>
+      <c r="G23" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1316,8 +1665,14 @@
       <c r="E24">
         <v>15642</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="F24" s="1">
+        <v>42345</v>
+      </c>
+      <c r="G24" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1333,8 +1688,14 @@
       <c r="E25">
         <v>40835</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="F25" s="1">
+        <v>42345</v>
+      </c>
+      <c r="G25" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1350,8 +1711,14 @@
       <c r="E26">
         <v>40951</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="F26" s="1">
+        <v>42345</v>
+      </c>
+      <c r="G26" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1367,8 +1734,14 @@
       <c r="E27">
         <v>19893</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="F27" s="1">
+        <v>42345</v>
+      </c>
+      <c r="G27" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1384,8 +1757,14 @@
       <c r="E28">
         <v>16395</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="F28" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G28" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1401,8 +1780,14 @@
       <c r="E29">
         <v>6582</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="F29" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G29" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1418,8 +1803,14 @@
       <c r="E30">
         <v>15907</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="F30" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G30" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1435,8 +1826,14 @@
       <c r="E31">
         <v>25297</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="F31" s="2">
+        <v>42346</v>
+      </c>
+      <c r="G31" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1452,8 +1849,14 @@
       <c r="E32">
         <v>8174</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G32" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1469,8 +1872,14 @@
       <c r="E33">
         <v>12600</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G33" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1486,8 +1895,14 @@
       <c r="E34">
         <v>9810</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G34" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1503,8 +1918,14 @@
       <c r="E35">
         <v>19290</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G35" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1520,8 +1941,14 @@
       <c r="E36">
         <v>23528</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G36" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1537,8 +1964,14 @@
       <c r="E37">
         <v>44957</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G37" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1554,8 +1987,14 @@
       <c r="E38">
         <v>8449</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G38" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>1</v>
       </c>
@@ -1571,8 +2010,14 @@
       <c r="E39">
         <v>2674</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G39" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>1</v>
       </c>
@@ -1588,8 +2033,14 @@
       <c r="E40">
         <v>12138</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G40" s="1">
+        <v>42376</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>1</v>
       </c>
@@ -1605,8 +2056,14 @@
       <c r="E41">
         <v>27675</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G41" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>1</v>
       </c>
@@ -1622,8 +2079,14 @@
       <c r="E42">
         <v>7159</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G42" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>1</v>
       </c>
@@ -1639,8 +2102,14 @@
       <c r="E43">
         <v>16680</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G43" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>1</v>
       </c>
@@ -1656,8 +2125,14 @@
       <c r="E44">
         <v>18395</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" s="1">
+        <v>42346</v>
+      </c>
+      <c r="G44" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>1</v>
       </c>
@@ -1673,8 +2148,14 @@
       <c r="E45">
         <v>13027</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" s="2">
+        <v>42346</v>
+      </c>
+      <c r="G45" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>1</v>
       </c>
@@ -1690,8 +2171,14 @@
       <c r="E46">
         <v>9432</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" s="2">
+        <v>42346</v>
+      </c>
+      <c r="G46" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>1</v>
       </c>
@@ -1707,8 +2194,14 @@
       <c r="E47">
         <v>41281</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" s="2">
+        <v>42346</v>
+      </c>
+      <c r="G47" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>1</v>
       </c>
@@ -1724,8 +2217,14 @@
       <c r="E48">
         <v>3537</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" s="2">
+        <v>42346</v>
+      </c>
+      <c r="G48" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>1</v>
       </c>
@@ -1741,8 +2240,14 @@
       <c r="E49">
         <v>3670</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="2">
+        <v>42348</v>
+      </c>
+      <c r="G49" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>1</v>
       </c>
@@ -1758,8 +2263,14 @@
       <c r="E50">
         <v>17616</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" s="2">
+        <v>42346</v>
+      </c>
+      <c r="G50" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>1</v>
       </c>
@@ -1775,8 +2286,14 @@
       <c r="E51">
         <v>8862</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" s="2">
+        <v>42348</v>
+      </c>
+      <c r="G51" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>1</v>
       </c>
@@ -1792,8 +2309,14 @@
       <c r="E52">
         <v>133315</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" s="1">
+        <v>42349</v>
+      </c>
+      <c r="G52" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>1</v>
       </c>
@@ -1809,8 +2332,14 @@
       <c r="E53">
         <v>30429</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" s="1">
+        <v>42349</v>
+      </c>
+      <c r="G53" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>1</v>
       </c>
@@ -1826,8 +2355,14 @@
       <c r="E54">
         <v>47214</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54" s="1">
+        <v>42349</v>
+      </c>
+      <c r="G54" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>1</v>
       </c>
@@ -1843,8 +2378,14 @@
       <c r="E55">
         <v>10876</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" s="1">
+        <v>42349</v>
+      </c>
+      <c r="G55" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>1</v>
       </c>
@@ -1860,8 +2401,14 @@
       <c r="E56">
         <v>78787</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56" s="1">
+        <v>42350</v>
+      </c>
+      <c r="G56" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>1</v>
       </c>
@@ -1877,8 +2424,14 @@
       <c r="E57">
         <v>23317</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57" s="1">
+        <v>42349</v>
+      </c>
+      <c r="G57" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>2</v>
       </c>
@@ -1894,8 +2447,14 @@
       <c r="E58">
         <v>7657</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58" s="1">
+        <v>42350</v>
+      </c>
+      <c r="G58" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>2</v>
       </c>
@@ -1911,8 +2470,14 @@
       <c r="E59">
         <v>6314</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59" s="1">
+        <v>42350</v>
+      </c>
+      <c r="G59" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>2</v>
       </c>
@@ -1928,8 +2493,14 @@
       <c r="E60">
         <v>5678</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60" s="1">
+        <v>42350</v>
+      </c>
+      <c r="G60" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>2</v>
       </c>
@@ -1945,8 +2516,14 @@
       <c r="E61">
         <v>1193</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61" s="1">
+        <v>42350</v>
+      </c>
+      <c r="G61" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>2</v>
       </c>
@@ -1962,8 +2539,14 @@
       <c r="E62">
         <v>42464</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62" s="1">
+        <v>42350</v>
+      </c>
+      <c r="G62" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63">
         <v>2</v>
       </c>
@@ -1979,8 +2562,14 @@
       <c r="E63">
         <v>2158</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63" s="1">
+        <v>42350</v>
+      </c>
+      <c r="G63" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64">
         <v>2</v>
       </c>
@@ -1996,8 +2585,14 @@
       <c r="E64">
         <v>14692</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64" s="1">
+        <v>42350</v>
+      </c>
+      <c r="G64" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>2</v>
       </c>
@@ -2013,8 +2608,14 @@
       <c r="E65">
         <v>38215</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65" s="1">
+        <v>42350</v>
+      </c>
+      <c r="G65" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>2</v>
       </c>
@@ -2030,8 +2631,14 @@
       <c r="E66">
         <v>18687</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="F66" s="1">
+        <v>42351</v>
+      </c>
+      <c r="G66" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>2</v>
       </c>
@@ -2047,8 +2654,14 @@
       <c r="E67">
         <v>18147</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67" s="1">
+        <v>42351</v>
+      </c>
+      <c r="G67" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>3</v>
       </c>
@@ -2064,8 +2677,14 @@
       <c r="E68">
         <v>3426</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="F68" s="1">
+        <v>42351</v>
+      </c>
+      <c r="G68" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>3</v>
       </c>
@@ -2081,8 +2700,14 @@
       <c r="E69">
         <v>34360</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="F69" s="1">
+        <v>42351</v>
+      </c>
+      <c r="G69" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>3</v>
       </c>
@@ -2098,8 +2723,14 @@
       <c r="E70">
         <v>6720</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="F70" s="1">
+        <v>42351</v>
+      </c>
+      <c r="G70" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71">
         <v>3</v>
       </c>
@@ -2115,8 +2746,14 @@
       <c r="E71">
         <v>3960</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="F71" s="1">
+        <v>42351</v>
+      </c>
+      <c r="G71" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72">
         <v>3</v>
       </c>
@@ -2132,8 +2769,14 @@
       <c r="E72">
         <v>5106</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="F72" s="1">
+        <v>42351</v>
+      </c>
+      <c r="G72" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73">
         <v>3</v>
       </c>
@@ -2149,8 +2792,14 @@
       <c r="E73">
         <v>20068</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="F73" s="1">
+        <v>42351</v>
+      </c>
+      <c r="G73" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74">
         <v>3</v>
       </c>
@@ -2166,8 +2815,14 @@
       <c r="E74">
         <v>1807</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="F74" s="1">
+        <v>42351</v>
+      </c>
+      <c r="G74" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75">
         <v>3</v>
       </c>
@@ -2183,8 +2838,14 @@
       <c r="E75">
         <v>11220</v>
       </c>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="F75" s="1">
+        <v>42352</v>
+      </c>
+      <c r="G75" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76">
         <v>3</v>
       </c>
@@ -2200,8 +2861,14 @@
       <c r="E76">
         <v>14</v>
       </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="F76" s="1">
+        <v>42352</v>
+      </c>
+      <c r="G76" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77">
         <v>3</v>
       </c>
@@ -2217,8 +2884,14 @@
       <c r="E77">
         <v>14637</v>
       </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="F77" s="1">
+        <v>42352</v>
+      </c>
+      <c r="G77" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78">
         <v>4</v>
       </c>
@@ -2234,8 +2907,14 @@
       <c r="E78">
         <v>57816</v>
       </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="F78" s="1">
+        <v>42352</v>
+      </c>
+      <c r="G78" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79">
         <v>5</v>
       </c>
@@ -2251,8 +2930,14 @@
       <c r="E79">
         <v>37645</v>
       </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="F79" s="1">
+        <v>42369</v>
+      </c>
+      <c r="G79" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80">
         <v>5</v>
       </c>
@@ -2268,8 +2953,14 @@
       <c r="E80">
         <v>3987</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="F80" s="1">
+        <v>42369</v>
+      </c>
+      <c r="G80" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81">
         <v>6</v>
       </c>
@@ -2288,8 +2979,11 @@
       <c r="F81" s="1">
         <v>42341</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="G81" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82">
         <v>7</v>
       </c>
@@ -2305,8 +2999,14 @@
       <c r="E82">
         <v>13815</v>
       </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="F82" s="1">
+        <v>42369</v>
+      </c>
+      <c r="G82" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83">
         <v>7</v>
       </c>
@@ -2322,8 +3022,14 @@
       <c r="E83">
         <v>11128</v>
       </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="F83" s="1">
+        <v>42369</v>
+      </c>
+      <c r="G83" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84">
         <v>7</v>
       </c>
@@ -2339,8 +3045,14 @@
       <c r="E84">
         <v>27206</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="F84" s="1">
+        <v>42369</v>
+      </c>
+      <c r="G84" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85">
         <v>7</v>
       </c>
@@ -2356,8 +3068,14 @@
       <c r="E85">
         <v>14087</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="F85" s="1">
+        <v>42369</v>
+      </c>
+      <c r="G85" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86">
         <v>7</v>
       </c>
@@ -2373,8 +3091,14 @@
       <c r="E86">
         <v>45757</v>
       </c>
-    </row>
-    <row r="87" spans="1:6">
+      <c r="F86" s="1">
+        <v>42369</v>
+      </c>
+      <c r="G86" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87">
         <v>7</v>
       </c>
@@ -2390,8 +3114,14 @@
       <c r="E87">
         <v>20657</v>
       </c>
-    </row>
-    <row r="88" spans="1:6">
+      <c r="F87" s="1">
+        <v>42369</v>
+      </c>
+      <c r="G87" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88">
         <v>7</v>
       </c>
@@ -2407,8 +3137,14 @@
       <c r="E88">
         <v>86528</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
+      <c r="F88" s="1">
+        <v>42369</v>
+      </c>
+      <c r="G88" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89">
         <v>7</v>
       </c>
@@ -2424,8 +3160,14 @@
       <c r="E89">
         <v>37023</v>
       </c>
-    </row>
-    <row r="90" spans="1:6">
+      <c r="F89" s="1">
+        <v>42369</v>
+      </c>
+      <c r="G89" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90">
         <v>7</v>
       </c>
@@ -2441,8 +3183,14 @@
       <c r="E90">
         <v>74672</v>
       </c>
-    </row>
-    <row r="91" spans="1:6">
+      <c r="F90" s="1">
+        <v>42369</v>
+      </c>
+      <c r="G90" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91">
         <v>7</v>
       </c>
@@ -2458,8 +3206,14 @@
       <c r="E91">
         <v>25546</v>
       </c>
-    </row>
-    <row r="92" spans="1:6">
+      <c r="F91" s="1">
+        <v>42369</v>
+      </c>
+      <c r="G91" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92">
         <v>7</v>
       </c>
@@ -2475,8 +3229,14 @@
       <c r="E92">
         <v>16131</v>
       </c>
-    </row>
-    <row r="93" spans="1:6">
+      <c r="F92" s="1">
+        <v>42369</v>
+      </c>
+      <c r="G92" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93">
         <v>7</v>
       </c>
@@ -2492,8 +3252,14 @@
       <c r="E93">
         <v>4618</v>
       </c>
-    </row>
-    <row r="94" spans="1:6">
+      <c r="F93" s="1">
+        <v>42369</v>
+      </c>
+      <c r="G93" s="1">
+        <v>42377</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94">
         <v>8</v>
       </c>
@@ -2509,8 +3275,14 @@
       <c r="E94">
         <v>16702</v>
       </c>
-    </row>
-    <row r="95" spans="1:6">
+      <c r="F94" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G94" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95">
         <v>8</v>
       </c>
@@ -2526,8 +3298,14 @@
       <c r="E95">
         <v>26968</v>
       </c>
-    </row>
-    <row r="96" spans="1:6">
+      <c r="F95" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G95" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96">
         <v>8</v>
       </c>
@@ -2543,8 +3321,14 @@
       <c r="E96">
         <v>51938</v>
       </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="F96" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G96" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97">
         <v>9</v>
       </c>
@@ -2560,8 +3344,14 @@
       <c r="E97">
         <v>11062</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="F97" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G97" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98">
         <v>9</v>
       </c>
@@ -2577,8 +3367,14 @@
       <c r="E98">
         <v>15578</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="F98" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G98" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99">
         <v>9</v>
       </c>
@@ -2594,8 +3390,14 @@
       <c r="E99">
         <v>2934</v>
       </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="F99" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G99" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100">
         <v>9</v>
       </c>
@@ -2611,8 +3413,14 @@
       <c r="E100">
         <v>423</v>
       </c>
-    </row>
-    <row r="101" spans="1:5">
+      <c r="F100" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G100" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101">
         <v>9</v>
       </c>
@@ -2628,8 +3436,14 @@
       <c r="E101">
         <v>15033</v>
       </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="F101" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G101" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102">
         <v>9</v>
       </c>
@@ -2645,8 +3459,14 @@
       <c r="E102">
         <v>296420</v>
       </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="F102" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G102" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103">
         <v>9</v>
       </c>
@@ -2662,8 +3482,14 @@
       <c r="E103">
         <v>6591</v>
       </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="F103" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G103" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104">
         <v>9</v>
       </c>
@@ -2679,8 +3505,14 @@
       <c r="E104">
         <v>125030</v>
       </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="F104" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G104" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105">
         <v>9</v>
       </c>
@@ -2696,8 +3528,14 @@
       <c r="E105">
         <v>21071</v>
       </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="F105" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G105" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106">
         <v>9</v>
       </c>
@@ -2713,8 +3551,14 @@
       <c r="E106">
         <v>44297</v>
       </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="F106" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G106" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107">
         <v>9</v>
       </c>
@@ -2730,8 +3574,14 @@
       <c r="E107">
         <v>37289</v>
       </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="F107" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G107" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
       <c r="A108">
         <v>9</v>
       </c>
@@ -2747,8 +3597,14 @@
       <c r="E108">
         <v>8192</v>
       </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="F108" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G108" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109">
         <v>9</v>
       </c>
@@ -2764,8 +3620,14 @@
       <c r="E109">
         <v>106262</v>
       </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="F109" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G109" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
       <c r="A110">
         <v>9</v>
       </c>
@@ -2781,8 +3643,14 @@
       <c r="E110">
         <v>29367</v>
       </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="F110" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G110" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111">
         <v>9</v>
       </c>
@@ -2798,8 +3666,14 @@
       <c r="E111">
         <v>6980</v>
       </c>
-    </row>
-    <row r="112" spans="1:5">
+      <c r="F111" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G111" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
       <c r="A112">
         <v>9</v>
       </c>
@@ -2815,8 +3689,14 @@
       <c r="E112">
         <v>938</v>
       </c>
-    </row>
-    <row r="113" spans="1:5">
+      <c r="F112" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G112" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
       <c r="A113">
         <v>9</v>
       </c>
@@ -2832,8 +3712,14 @@
       <c r="E113">
         <v>2779</v>
       </c>
-    </row>
-    <row r="114" spans="1:5">
+      <c r="F113" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G113" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
       <c r="A114">
         <v>9</v>
       </c>
@@ -2849,8 +3735,14 @@
       <c r="E114">
         <v>2076</v>
       </c>
-    </row>
-    <row r="115" spans="1:5">
+      <c r="F114" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G114" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
       <c r="A115">
         <v>9</v>
       </c>
@@ -2866,8 +3758,14 @@
       <c r="E115">
         <v>81</v>
       </c>
-    </row>
-    <row r="116" spans="1:5">
+      <c r="F115" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G115" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
       <c r="A116">
         <v>9</v>
       </c>
@@ -2883,8 +3781,14 @@
       <c r="E116">
         <v>168722</v>
       </c>
-    </row>
-    <row r="117" spans="1:5">
+      <c r="F116" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G116" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
       <c r="A117">
         <v>9</v>
       </c>
@@ -2900,8 +3804,14 @@
       <c r="E117">
         <v>12859</v>
       </c>
-    </row>
-    <row r="118" spans="1:5">
+      <c r="F117" s="1">
+        <v>42370</v>
+      </c>
+      <c r="G117" s="1">
+        <v>42378</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
       <c r="A118">
         <v>9</v>
       </c>
@@ -2917,8 +3827,14 @@
       <c r="E118">
         <v>3</v>
       </c>
-    </row>
-    <row r="119" spans="1:5">
+      <c r="F118" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G118" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
       <c r="A119">
         <v>99</v>
       </c>
@@ -2934,8 +3850,15 @@
       <c r="E119">
         <v>36</v>
       </c>
+      <c r="F119" s="1">
+        <v>42371</v>
+      </c>
+      <c r="G119" s="1">
+        <v>42378</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Change the algorithm of constrained optimization in simulation
1. Separate regression analysis and summary statistics from income
effect.
2. Rather than using ConstrOptim for simulating expenditure share, we
switch to nloptr, which is a better optimizer.
3. Add one version of estimation and simulation: v1 — old version where
the inclusive value is 1d spline in expenditure and change in discrete
income level; v2 — 2-dimensional gam spline model.
</commit_message>
<xml_diff>
--- a/SAS/Retail_attributes_RMS/retail_attributes_rms_log.xlsx
+++ b/SAS/Retail_attributes_RMS/retail_attributes_rms_log.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19100" tabRatio="500"/>
+    <workbookView xWindow="1080" yWindow="0" windowWidth="25600" windowHeight="19100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="126">
   <si>
     <t>department_code</t>
   </si>
@@ -391,6 +391,12 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>NOTE:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. UPC_weight 5520_2006.csv is generated using the 2007 data. </t>
   </si>
 </sst>
 </file>
@@ -452,8 +458,104 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="129">
+  <cellStyleXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -588,7 +690,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="129">
+  <cellStyles count="225">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -653,6 +755,54 @@
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -717,6 +867,54 @@
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1046,11 +1244,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K119"/>
+  <dimension ref="A1:K125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -1114,6 +1310,15 @@
       <c r="H2" s="1">
         <v>42378</v>
       </c>
+      <c r="I2" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J2" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K2" s="1">
+        <v>42384</v>
+      </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
@@ -1140,6 +1345,15 @@
       <c r="H3" s="1">
         <v>42378</v>
       </c>
+      <c r="I3" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J3" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K3" s="1">
+        <v>42384</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
@@ -1166,6 +1380,15 @@
       <c r="H4" s="1">
         <v>42378</v>
       </c>
+      <c r="I4" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J4" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K4" s="1">
+        <v>42384</v>
+      </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
@@ -1192,6 +1415,15 @@
       <c r="H5" s="1">
         <v>42378</v>
       </c>
+      <c r="I5" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J5" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K5" s="1">
+        <v>42384</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
@@ -1218,6 +1450,15 @@
       <c r="H6" s="1">
         <v>42378</v>
       </c>
+      <c r="I6" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J6" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K6" s="1">
+        <v>42384</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
@@ -1244,6 +1485,15 @@
       <c r="H7" s="1">
         <v>42378</v>
       </c>
+      <c r="I7" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J7" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K7" s="1">
+        <v>42384</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
@@ -1270,6 +1520,15 @@
       <c r="H8" s="1">
         <v>42378</v>
       </c>
+      <c r="I8" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J8" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K8" s="1">
+        <v>42384</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9">
@@ -1296,6 +1555,15 @@
       <c r="H9" s="1">
         <v>42378</v>
       </c>
+      <c r="I9" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J9" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K9" s="1">
+        <v>42384</v>
+      </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10">
@@ -1322,6 +1590,15 @@
       <c r="H10" s="1">
         <v>42378</v>
       </c>
+      <c r="I10" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J10" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K10" s="1">
+        <v>42384</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11">
@@ -1348,6 +1625,15 @@
       <c r="H11" s="1">
         <v>42378</v>
       </c>
+      <c r="I11" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J11" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K11" s="1">
+        <v>42384</v>
+      </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12">
@@ -1374,6 +1660,15 @@
       <c r="H12" s="1">
         <v>42379</v>
       </c>
+      <c r="I12" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J12" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K12" s="1">
+        <v>42384</v>
+      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13">
@@ -1400,6 +1695,15 @@
       <c r="H13" s="1">
         <v>42379</v>
       </c>
+      <c r="I13" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J13" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K13" s="1">
+        <v>42384</v>
+      </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14">
@@ -1426,6 +1730,15 @@
       <c r="H14" s="1">
         <v>42379</v>
       </c>
+      <c r="I14" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J14" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K14" s="1">
+        <v>42384</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15">
@@ -1452,6 +1765,15 @@
       <c r="H15" s="1">
         <v>42379</v>
       </c>
+      <c r="I15" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J15" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K15" s="1">
+        <v>42384</v>
+      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16">
@@ -1478,8 +1800,17 @@
       <c r="H16" s="1">
         <v>42379</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J16" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K16" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>0</v>
       </c>
@@ -1504,8 +1835,17 @@
       <c r="H17" s="1">
         <v>42379</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J17" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K17" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1530,8 +1870,17 @@
       <c r="H18" s="1">
         <v>42379</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J18" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K18" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>0</v>
       </c>
@@ -1556,8 +1905,17 @@
       <c r="H19" s="1">
         <v>42379</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J19" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K19" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1579,8 +1937,20 @@
       <c r="G20" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="H20" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I20" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J20" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K20" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1602,8 +1972,20 @@
       <c r="G21" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="H21" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I21" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J21" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K21" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1625,8 +2007,20 @@
       <c r="G22" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="H22" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I22" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J22" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K22" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1648,8 +2042,20 @@
       <c r="G23" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="H23" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I23" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J23" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K23" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1671,8 +2077,20 @@
       <c r="G24" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="H24" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I24" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J24" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K24" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1694,8 +2112,20 @@
       <c r="G25" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="H25" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I25" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J25" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K25" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1717,8 +2147,20 @@
       <c r="G26" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="H26" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I26" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J26" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K26" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1740,8 +2182,20 @@
       <c r="G27" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="H27" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I27" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J27" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K27" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1763,8 +2217,20 @@
       <c r="G28" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="H28" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I28" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J28" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K28" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1786,8 +2252,20 @@
       <c r="G29" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="H29" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I29" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J29" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K29" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1809,8 +2287,20 @@
       <c r="G30" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="H30" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I30" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J30" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K30" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1832,8 +2322,20 @@
       <c r="G31" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="H31" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I31" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J31" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K31" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1855,8 +2357,20 @@
       <c r="G32" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I32" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J32" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K32" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1878,8 +2392,20 @@
       <c r="G33" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I33" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J33" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K33" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1901,8 +2427,20 @@
       <c r="G34" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I34" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J34" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K34" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1924,8 +2462,20 @@
       <c r="G35" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I35" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J35" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K35" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1947,8 +2497,20 @@
       <c r="G36" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I36" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J36" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K36" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1970,8 +2532,20 @@
       <c r="G37" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I37" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J37" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K37" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1993,8 +2567,20 @@
       <c r="G38" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H38" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I38" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J38" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K38" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2016,8 +2602,20 @@
       <c r="G39" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="H39" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I39" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J39" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K39" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>1</v>
       </c>
@@ -2039,8 +2637,20 @@
       <c r="G40" s="1">
         <v>42376</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="H40" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I40" s="1">
+        <v>42381</v>
+      </c>
+      <c r="J40" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K40" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>1</v>
       </c>
@@ -2062,8 +2672,20 @@
       <c r="G41" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="H41" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I41" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J41" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K41" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>1</v>
       </c>
@@ -2085,8 +2707,20 @@
       <c r="G42" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="H42" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I42" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J42" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K42" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>1</v>
       </c>
@@ -2108,8 +2742,20 @@
       <c r="G43" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="H43" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I43" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J43" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K43" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>1</v>
       </c>
@@ -2131,8 +2777,20 @@
       <c r="G44" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="H44" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I44" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J44" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K44" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45">
         <v>1</v>
       </c>
@@ -2154,8 +2812,20 @@
       <c r="G45" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="H45" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I45" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J45" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K45" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46">
         <v>1</v>
       </c>
@@ -2177,8 +2847,20 @@
       <c r="G46" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="H46" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I46" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J46" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K46" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47">
         <v>1</v>
       </c>
@@ -2200,8 +2882,20 @@
       <c r="G47" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="H47" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I47" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J47" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K47" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48">
         <v>1</v>
       </c>
@@ -2223,8 +2917,20 @@
       <c r="G48" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="H48" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I48" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J48" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K48" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49">
         <v>1</v>
       </c>
@@ -2246,8 +2952,20 @@
       <c r="G49" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="H49" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I49" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J49" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K49" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50">
         <v>1</v>
       </c>
@@ -2269,8 +2987,20 @@
       <c r="G50" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="H50" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I50" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J50" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K50" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51">
         <v>1</v>
       </c>
@@ -2292,8 +3022,20 @@
       <c r="G51" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="H51" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I51" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J51" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K51" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52">
         <v>1</v>
       </c>
@@ -2315,8 +3057,20 @@
       <c r="G52" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="H52" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I52" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J52" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K52" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53">
         <v>1</v>
       </c>
@@ -2338,8 +3092,20 @@
       <c r="G53" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="H53" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I53" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J53" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K53" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54">
         <v>1</v>
       </c>
@@ -2361,8 +3127,20 @@
       <c r="G54" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="H54" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I54" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J54" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K54" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55">
         <v>1</v>
       </c>
@@ -2384,8 +3162,20 @@
       <c r="G55" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="H55" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I55" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J55" s="1">
+        <v>42383</v>
+      </c>
+      <c r="K55" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56">
         <v>1</v>
       </c>
@@ -2407,8 +3197,20 @@
       <c r="G56" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="H56" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I56" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J56" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K56" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57">
         <v>1</v>
       </c>
@@ -2430,8 +3232,20 @@
       <c r="G57" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="H57" s="1">
+        <v>42379</v>
+      </c>
+      <c r="I57" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J57" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K57" s="1">
+        <v>42384</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58">
         <v>2</v>
       </c>
@@ -2453,8 +3267,20 @@
       <c r="G58" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="H58" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I58" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J58" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K58" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59">
         <v>2</v>
       </c>
@@ -2476,8 +3302,20 @@
       <c r="G59" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="60" spans="1:7">
+      <c r="H59" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I59" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J59" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K59" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60">
         <v>2</v>
       </c>
@@ -2499,8 +3337,20 @@
       <c r="G60" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="H60" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I60" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J60" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K60" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61">
         <v>2</v>
       </c>
@@ -2522,8 +3372,20 @@
       <c r="G61" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="62" spans="1:7">
+      <c r="H61" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I61" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J61" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K61" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62">
         <v>2</v>
       </c>
@@ -2545,8 +3407,20 @@
       <c r="G62" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="63" spans="1:7">
+      <c r="H62" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I62" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J62" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K62" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63">
         <v>2</v>
       </c>
@@ -2568,8 +3442,20 @@
       <c r="G63" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="64" spans="1:7">
+      <c r="H63" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I63" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J63" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K63" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64">
         <v>2</v>
       </c>
@@ -2591,8 +3477,20 @@
       <c r="G64" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="65" spans="1:7">
+      <c r="H64" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I64" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J64" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K64" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65">
         <v>2</v>
       </c>
@@ -2614,8 +3512,20 @@
       <c r="G65" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="66" spans="1:7">
+      <c r="H65" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I65" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J65" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K65" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66">
         <v>2</v>
       </c>
@@ -2637,8 +3547,20 @@
       <c r="G66" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="67" spans="1:7">
+      <c r="H66" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I66" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J66" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K66" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67">
         <v>2</v>
       </c>
@@ -2660,8 +3582,20 @@
       <c r="G67" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="68" spans="1:7">
+      <c r="H67" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I67" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J67" s="2">
+        <v>42383</v>
+      </c>
+      <c r="K67" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68">
         <v>3</v>
       </c>
@@ -2683,8 +3617,20 @@
       <c r="G68" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="69" spans="1:7">
+      <c r="H68" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I68" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J68" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K68" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69">
         <v>3</v>
       </c>
@@ -2706,8 +3652,20 @@
       <c r="G69" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="70" spans="1:7">
+      <c r="H69" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I69" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J69" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K69" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70">
         <v>3</v>
       </c>
@@ -2729,8 +3687,20 @@
       <c r="G70" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="71" spans="1:7">
+      <c r="H70" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I70" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J70" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K70" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71">
         <v>3</v>
       </c>
@@ -2752,8 +3722,20 @@
       <c r="G71" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="72" spans="1:7">
+      <c r="H71" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I71" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J71" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K71" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72">
         <v>3</v>
       </c>
@@ -2775,8 +3757,20 @@
       <c r="G72" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="73" spans="1:7">
+      <c r="H72" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I72" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J72" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K72" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73">
         <v>3</v>
       </c>
@@ -2798,8 +3792,20 @@
       <c r="G73" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="74" spans="1:7">
+      <c r="H73" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I73" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J73" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K73" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74">
         <v>3</v>
       </c>
@@ -2821,8 +3827,20 @@
       <c r="G74" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="75" spans="1:7">
+      <c r="H74" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I74" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J74" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K74" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
       <c r="A75">
         <v>3</v>
       </c>
@@ -2844,8 +3862,20 @@
       <c r="G75" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="76" spans="1:7">
+      <c r="H75" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I75" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J75" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K75" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76">
         <v>3</v>
       </c>
@@ -2867,8 +3897,20 @@
       <c r="G76" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="77" spans="1:7">
+      <c r="H76" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I76" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J76" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K76" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77">
         <v>3</v>
       </c>
@@ -2890,8 +3932,20 @@
       <c r="G77" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="78" spans="1:7">
+      <c r="H77" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I77" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J77" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K77" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78">
         <v>4</v>
       </c>
@@ -2913,8 +3967,20 @@
       <c r="G78" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="79" spans="1:7">
+      <c r="H78" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I78" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J78" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K78" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79">
         <v>5</v>
       </c>
@@ -2936,8 +4002,20 @@
       <c r="G79" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="80" spans="1:7">
+      <c r="H79" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I79" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J79" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K79" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80">
         <v>5</v>
       </c>
@@ -2959,8 +4037,20 @@
       <c r="G80" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="81" spans="1:7">
+      <c r="H80" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I80" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J80" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K80" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
       <c r="A81">
         <v>6</v>
       </c>
@@ -2982,8 +4072,20 @@
       <c r="G81" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="82" spans="1:7">
+      <c r="H81" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I81" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J81" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K81" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
       <c r="A82">
         <v>7</v>
       </c>
@@ -3005,8 +4107,20 @@
       <c r="G82" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="83" spans="1:7">
+      <c r="H82" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I82" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J82" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K82" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83">
         <v>7</v>
       </c>
@@ -3028,8 +4142,20 @@
       <c r="G83" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="84" spans="1:7">
+      <c r="H83" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I83" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J83" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K83" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84">
         <v>7</v>
       </c>
@@ -3051,8 +4177,20 @@
       <c r="G84" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="85" spans="1:7">
+      <c r="H84" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I84" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J84" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K84" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
       <c r="A85">
         <v>7</v>
       </c>
@@ -3074,8 +4212,20 @@
       <c r="G85" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="86" spans="1:7">
+      <c r="H85" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I85" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J85" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K85" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
       <c r="A86">
         <v>7</v>
       </c>
@@ -3097,8 +4247,20 @@
       <c r="G86" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="87" spans="1:7">
+      <c r="H86" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I86" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J86" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K86" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
       <c r="A87">
         <v>7</v>
       </c>
@@ -3120,8 +4282,20 @@
       <c r="G87" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="88" spans="1:7">
+      <c r="H87" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I87" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J87" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K87" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
       <c r="A88">
         <v>7</v>
       </c>
@@ -3143,8 +4317,20 @@
       <c r="G88" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="89" spans="1:7">
+      <c r="H88" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I88" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J88" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K88" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
       <c r="A89">
         <v>7</v>
       </c>
@@ -3166,8 +4352,20 @@
       <c r="G89" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="90" spans="1:7">
+      <c r="H89" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I89" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J89" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K89" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
       <c r="A90">
         <v>7</v>
       </c>
@@ -3189,8 +4387,20 @@
       <c r="G90" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="91" spans="1:7">
+      <c r="H90" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I90" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J90" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K90" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
       <c r="A91">
         <v>7</v>
       </c>
@@ -3212,8 +4422,20 @@
       <c r="G91" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="92" spans="1:7">
+      <c r="H91" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I91" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J91" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K91" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
       <c r="A92">
         <v>7</v>
       </c>
@@ -3235,8 +4457,20 @@
       <c r="G92" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="93" spans="1:7">
+      <c r="H92" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I92" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J92" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K92" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
       <c r="A93">
         <v>7</v>
       </c>
@@ -3258,8 +4492,20 @@
       <c r="G93" s="1">
         <v>42377</v>
       </c>
-    </row>
-    <row r="94" spans="1:7">
+      <c r="H93" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I93" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J93" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K93" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
       <c r="A94">
         <v>8</v>
       </c>
@@ -3281,8 +4527,20 @@
       <c r="G94" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="95" spans="1:7">
+      <c r="H94" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I94" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J94" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K94" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
       <c r="A95">
         <v>8</v>
       </c>
@@ -3304,8 +4562,20 @@
       <c r="G95" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="96" spans="1:7">
+      <c r="H95" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I95" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J95" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K95" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
       <c r="A96">
         <v>8</v>
       </c>
@@ -3327,8 +4597,20 @@
       <c r="G96" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="97" spans="1:7">
+      <c r="H96" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I96" s="1">
+        <v>42382</v>
+      </c>
+      <c r="J96" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K96" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
       <c r="A97">
         <v>9</v>
       </c>
@@ -3350,8 +4632,20 @@
       <c r="G97" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="98" spans="1:7">
+      <c r="H97" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I97" s="1">
+        <v>42383</v>
+      </c>
+      <c r="J97" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K97" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="A98">
         <v>9</v>
       </c>
@@ -3373,8 +4667,20 @@
       <c r="G98" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="99" spans="1:7">
+      <c r="H98" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I98" s="1">
+        <v>42383</v>
+      </c>
+      <c r="J98" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K98" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
       <c r="A99">
         <v>9</v>
       </c>
@@ -3396,8 +4702,20 @@
       <c r="G99" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="100" spans="1:7">
+      <c r="H99" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I99" s="1">
+        <v>42383</v>
+      </c>
+      <c r="J99" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K99" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
       <c r="A100">
         <v>9</v>
       </c>
@@ -3419,8 +4737,20 @@
       <c r="G100" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="101" spans="1:7">
+      <c r="H100" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I100" s="1">
+        <v>42383</v>
+      </c>
+      <c r="J100" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K100" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
       <c r="A101">
         <v>9</v>
       </c>
@@ -3442,8 +4772,20 @@
       <c r="G101" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="102" spans="1:7">
+      <c r="H101" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I101" s="1">
+        <v>42383</v>
+      </c>
+      <c r="J101" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K101" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
       <c r="A102">
         <v>9</v>
       </c>
@@ -3465,8 +4807,20 @@
       <c r="G102" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="103" spans="1:7">
+      <c r="H102" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I102" s="1">
+        <v>42383</v>
+      </c>
+      <c r="J102" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K102" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
       <c r="A103">
         <v>9</v>
       </c>
@@ -3488,8 +4842,20 @@
       <c r="G103" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="104" spans="1:7">
+      <c r="H103" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I103" s="1">
+        <v>42383</v>
+      </c>
+      <c r="J103" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K103" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
       <c r="A104">
         <v>9</v>
       </c>
@@ -3511,8 +4877,20 @@
       <c r="G104" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="105" spans="1:7">
+      <c r="H104" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I104" s="1">
+        <v>42383</v>
+      </c>
+      <c r="J104" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K104" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
       <c r="A105">
         <v>9</v>
       </c>
@@ -3534,8 +4912,20 @@
       <c r="G105" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="106" spans="1:7">
+      <c r="H105" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I105" s="1">
+        <v>42383</v>
+      </c>
+      <c r="J105" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K105" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
       <c r="A106">
         <v>9</v>
       </c>
@@ -3557,8 +4947,20 @@
       <c r="G106" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="107" spans="1:7">
+      <c r="H106" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I106" s="1">
+        <v>42383</v>
+      </c>
+      <c r="J106" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K106" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
       <c r="A107">
         <v>9</v>
       </c>
@@ -3580,8 +4982,20 @@
       <c r="G107" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="108" spans="1:7">
+      <c r="H107" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I107" s="1">
+        <v>42383</v>
+      </c>
+      <c r="J107" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K107" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
       <c r="A108">
         <v>9</v>
       </c>
@@ -3603,8 +5017,20 @@
       <c r="G108" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="109" spans="1:7">
+      <c r="H108" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I108" s="2">
+        <v>42383</v>
+      </c>
+      <c r="J108" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K108" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
       <c r="A109">
         <v>9</v>
       </c>
@@ -3626,8 +5052,20 @@
       <c r="G109" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="110" spans="1:7">
+      <c r="H109" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I109" s="2">
+        <v>42383</v>
+      </c>
+      <c r="J109" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K109" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
       <c r="A110">
         <v>9</v>
       </c>
@@ -3649,8 +5087,20 @@
       <c r="G110" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="111" spans="1:7">
+      <c r="H110" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I110" s="2">
+        <v>42383</v>
+      </c>
+      <c r="J110" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K110" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
       <c r="A111">
         <v>9</v>
       </c>
@@ -3672,8 +5122,20 @@
       <c r="G111" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="112" spans="1:7">
+      <c r="H111" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I111" s="2">
+        <v>42383</v>
+      </c>
+      <c r="J111" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K111" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
       <c r="A112">
         <v>9</v>
       </c>
@@ -3695,8 +5157,20 @@
       <c r="G112" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="113" spans="1:7">
+      <c r="H112" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I112" s="2">
+        <v>42383</v>
+      </c>
+      <c r="J112" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K112" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
       <c r="A113">
         <v>9</v>
       </c>
@@ -3718,8 +5192,20 @@
       <c r="G113" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="114" spans="1:7">
+      <c r="H113" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I113" s="2">
+        <v>42383</v>
+      </c>
+      <c r="J113" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K113" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
       <c r="A114">
         <v>9</v>
       </c>
@@ -3741,8 +5227,20 @@
       <c r="G114" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="115" spans="1:7">
+      <c r="H114" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I114" s="2">
+        <v>42383</v>
+      </c>
+      <c r="J114" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K114" s="1">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11">
       <c r="A115">
         <v>9</v>
       </c>
@@ -3764,8 +5262,20 @@
       <c r="G115" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="116" spans="1:7">
+      <c r="H115" t="s">
+        <v>123</v>
+      </c>
+      <c r="I115" t="s">
+        <v>123</v>
+      </c>
+      <c r="J115" t="s">
+        <v>123</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11">
       <c r="A116">
         <v>9</v>
       </c>
@@ -3787,8 +5297,20 @@
       <c r="G116" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="117" spans="1:7">
+      <c r="H116" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I116" s="2">
+        <v>42383</v>
+      </c>
+      <c r="J116" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K116" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
       <c r="A117">
         <v>9</v>
       </c>
@@ -3810,8 +5332,20 @@
       <c r="G117" s="1">
         <v>42378</v>
       </c>
-    </row>
-    <row r="118" spans="1:7">
+      <c r="H117" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I117" s="2">
+        <v>42383</v>
+      </c>
+      <c r="J117" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K117" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11">
       <c r="A118">
         <v>9</v>
       </c>
@@ -3833,8 +5367,20 @@
       <c r="G118" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="119" spans="1:7">
+      <c r="H118" t="s">
+        <v>123</v>
+      </c>
+      <c r="I118" t="s">
+        <v>123</v>
+      </c>
+      <c r="J118" t="s">
+        <v>123</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11">
       <c r="A119">
         <v>99</v>
       </c>
@@ -3855,6 +5401,28 @@
       </c>
       <c r="G119" s="1">
         <v>42378</v>
+      </c>
+      <c r="H119" s="1">
+        <v>42380</v>
+      </c>
+      <c r="I119" s="1">
+        <v>42383</v>
+      </c>
+      <c r="J119" s="1">
+        <v>42384</v>
+      </c>
+      <c r="K119" s="1">
+        <v>42386</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
+      <c r="A124" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
+      <c r="A125" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>